<commit_message>
Stark settlement dc parser fails outside supply
Fails if bill is outside supply.
</commit_message>
<xml_diff>
--- a/test/electricity/bills.settlement.dc.stark.xlsx
+++ b/test/electricity/bills.settlement.dc.stark.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t xml:space="preserve">Date: 02/05/2018 09:17:38</t>
   </si>
@@ -205,8 +205,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,212 +247,313 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A7:AF12"/>
+  <dimension ref="A7:AF13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="S11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="U11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="W11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="X11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y11" s="1" t="s">
+      <c r="Y11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="1" t="s">
+      <c r="Z11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AA11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AB11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AC11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AD11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AE11" s="1" t="s">
+      <c r="AE11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AF11" s="1" t="s">
+      <c r="AF11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="3" t="n">
         <v>1472066139971</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="4" t="n">
         <v>43252</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="4" t="n">
         <v>43281</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="G12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="I12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="0" t="n">
+      <c r="I12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="n">
         <v>142.48</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="1" t="n">
         <v>11.87</v>
       </c>
-      <c r="M12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" s="0" t="n">
+      <c r="M12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1" t="n">
         <v>50.5</v>
       </c>
-      <c r="U12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="W12" s="0" t="n">
+      <c r="U12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W12" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="X12" s="0" t="n">
+      <c r="X12" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="Y12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="0" t="n">
+      <c r="Y12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="AD12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="4" t="n">
+      <c r="AD12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="5" t="n">
         <v>43264</v>
       </c>
-      <c r="AF12" s="0" t="n">
+      <c r="AF12" s="1" t="n">
+        <v>26.87</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>1472066139971</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>29738</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>29767</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>142.48</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="U13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W13" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="X13" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="AD13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="5" t="n">
+        <v>43264</v>
+      </c>
+      <c r="AF13" s="1" t="n">
         <v>26.87</v>
       </c>
     </row>

</xml_diff>